<commit_message>
Sales return upload and combo box details
</commit_message>
<xml_diff>
--- a/assets/templates/Sales_upload_format.xlsx
+++ b/assets/templates/Sales_upload_format.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t>Creation Date</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Box Name</t>
+  </si>
+  <si>
+    <t>Combo Box Name</t>
   </si>
 </sst>
 </file>
@@ -750,7 +753,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -763,9 +766,10 @@
     <col min="9" max="9" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="49.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -786,6 +790,9 @@
       </c>
       <c r="M1" t="s">
         <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>